<commit_message>
adding features for grouping regions
</commit_message>
<xml_diff>
--- a/notebooks/basic_dataset/Pril-Region_Pokaz_2024/Раздел 8 - Валовой региональный продукт.xlsx
+++ b/notebooks/basic_dataset/Pril-Region_Pokaz_2024/Раздел 8 - Валовой региональный продукт.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Диана\учеба 5 сем\пп\Environmental-monitoring-of-water-resources\notebooks\merge\Pril-Region_Pokaz_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Диана\учеба 5 сем\пп\Environmental-monitoring-of-water-resources\notebooks\basic_dataset\Pril-Region_Pokaz_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A931BF-BF8C-4AC1-BDB3-F5A4031C7BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932ECFA5-7688-4215-917C-EB327FA908CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5208" yWindow="1476" windowWidth="14244" windowHeight="10776" tabRatio="896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Раздел 8" sheetId="68" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="192">
   <si>
     <t>Белгородская область</t>
   </si>
@@ -2492,7 +2492,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2660,7 +2660,7 @@
   </sheetPr>
   <dimension ref="A1:Z109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
@@ -10015,11 +10015,11 @@
   </sheetPr>
   <dimension ref="A1:X106"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B93" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="8" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="Z94" sqref="Z94"/>
+      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12018,15 +12018,9 @@
       <c r="A32" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="73" t="s">
-        <v>97</v>
-      </c>
+      <c r="B32" s="73"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
       <c r="E32" s="73">
         <v>599201.69999999995</v>
       </c>
@@ -13716,21 +13710,11 @@
       <c r="A56" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="D56" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="E56" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="F56" s="73" t="s">
-        <v>97</v>
-      </c>
+      <c r="B56" s="73"/>
+      <c r="C56" s="73"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="73"/>
+      <c r="F56" s="73"/>
       <c r="G56" s="73">
         <v>20038.400000000001</v>
       </c>
@@ -15298,15 +15282,9 @@
       <c r="A78" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="B78" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="C78" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="D78" s="73" t="s">
-        <v>97</v>
-      </c>
+      <c r="B78" s="73"/>
+      <c r="C78" s="73"/>
+      <c r="D78" s="73"/>
       <c r="E78" s="73">
         <v>496127.8</v>
       </c>
@@ -15372,15 +15350,9 @@
       <c r="A79" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B79" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="C79" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="D79" s="73" t="s">
-        <v>97</v>
-      </c>
+      <c r="B79" s="73"/>
+      <c r="C79" s="73"/>
+      <c r="D79" s="73"/>
       <c r="E79" s="73">
         <v>555559.1</v>
       </c>

</xml_diff>